<commit_message>
Updated repot documents and users questionnaires
</commit_message>
<xml_diff>
--- a/documentation/user-experience-questionnaires/results/User Experience Questionnaire-1.xlsx
+++ b/documentation/user-experience-questionnaires/results/User Experience Questionnaire-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielcastro/Faculdade/Mestrado/1-ano/semestre-1/RVA/entrega-2-2021/WebXR-Furniture-Assembly/documentation/user-experience-questionnaires/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC657FC-175C-4548-8F71-5E635D6CF6F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C81E74-4502-494E-9E48-DB3A84530285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{09BE7136-0DDB-C649-AF3B-98935C3C9DEF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{09BE7136-0DDB-C649-AF3B-98935C3C9DEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="76">
   <si>
     <t>annoying</t>
   </si>
@@ -243,13 +243,25 @@
     <t>answer (0-1)</t>
   </si>
   <si>
-    <t>min total</t>
-  </si>
-  <si>
-    <t>max total</t>
-  </si>
-  <si>
-    <t>total</t>
+    <t>total (1-7)</t>
+  </si>
+  <si>
+    <t>max total (0-1)</t>
+  </si>
+  <si>
+    <t>total (0-1)</t>
+  </si>
+  <si>
+    <t>max total (1-7)</t>
+  </si>
+  <si>
+    <t>min total (1-7)</t>
+  </si>
+  <si>
+    <t>min total (0-1)</t>
+  </si>
+  <si>
+    <t>total (0-1) %</t>
   </si>
 </sst>
 </file>
@@ -310,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -322,7 +334,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -643,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07AA2E4F-3854-9D42-B3E7-9C4387E43AB7}">
-  <dimension ref="A1:O46"/>
+  <dimension ref="A1:Q46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -659,14 +670,17 @@
     <col min="6" max="6" width="15.1640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="14.6640625" style="1" customWidth="1"/>
     <col min="8" max="9" width="10.83203125" style="4"/>
-    <col min="10" max="10" width="22.1640625" style="7" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" style="7" customWidth="1"/>
-    <col min="12" max="13" width="14.33203125" style="7" customWidth="1"/>
-    <col min="14" max="14" width="16.1640625" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="10.83203125" style="4"/>
+    <col min="10" max="10" width="22.1640625" style="6" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" style="6" customWidth="1"/>
+    <col min="12" max="13" width="14.33203125" style="6" customWidth="1"/>
+    <col min="14" max="14" width="13.6640625" style="6" customWidth="1"/>
+    <col min="15" max="15" width="14.33203125" style="6" customWidth="1"/>
+    <col min="16" max="16" width="10.83203125" style="4"/>
+    <col min="17" max="17" width="13.6640625" style="4" customWidth="1"/>
+    <col min="18" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
@@ -690,17 +704,28 @@
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="N1" s="2"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q1" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -723,25 +748,37 @@
       <c r="G2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="7">
+      <c r="K2" s="6">
         <f>1*6</f>
         <v>6</v>
       </c>
-      <c r="L2" s="7">
-        <f>7*6</f>
+      <c r="L2" s="6">
+        <f>6*7</f>
         <v>42</v>
       </c>
       <c r="M2" s="3">
         <f>SUM(C2:C7)</f>
         <v>28</v>
       </c>
-      <c r="N2" s="3"/>
-      <c r="O2" s="5"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N2" s="3">
+        <v>0</v>
+      </c>
+      <c r="O2" s="3">
+        <v>6</v>
+      </c>
+      <c r="P2" s="3">
+        <f>SUM(E2:E7)</f>
+        <v>3.6666666666666665</v>
+      </c>
+      <c r="Q2" s="3">
+        <f>(SUM(E2:E7))/O2</f>
+        <v>0.61111111111111105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -764,14 +801,14 @@
       <c r="G3" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="6">
         <f>4*1</f>
         <v>4</v>
       </c>
-      <c r="L3" s="7">
+      <c r="L3" s="6">
         <f>4*7</f>
         <v>28</v>
       </c>
@@ -779,9 +816,22 @@
         <f>(SUM(C8:C11))</f>
         <v>25</v>
       </c>
-      <c r="N3" s="3"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N3" s="3">
+        <v>0</v>
+      </c>
+      <c r="O3" s="3">
+        <v>4</v>
+      </c>
+      <c r="P3" s="3">
+        <f>(SUM(E8:E11))</f>
+        <v>3.5000000000000004</v>
+      </c>
+      <c r="Q3" s="3">
+        <f>(SUM(E8:E11))/4</f>
+        <v>0.87500000000000011</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -804,14 +854,14 @@
       <c r="G4" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="6">
         <f>4*1</f>
         <v>4</v>
       </c>
-      <c r="L4" s="7">
+      <c r="L4" s="6">
         <f>4*7</f>
         <v>28</v>
       </c>
@@ -819,9 +869,22 @@
         <f>(SUM(C12:C15))</f>
         <v>27</v>
       </c>
-      <c r="N4" s="3"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N4" s="3">
+        <v>0</v>
+      </c>
+      <c r="O4" s="3">
+        <v>4</v>
+      </c>
+      <c r="P4" s="3">
+        <f>(SUM(E12:E15))</f>
+        <v>3.8333333333333335</v>
+      </c>
+      <c r="Q4" s="3">
+        <f>(SUM(E12:E15))/4</f>
+        <v>0.95833333333333337</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -844,14 +907,14 @@
       <c r="G5" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="6">
         <f>4*1</f>
         <v>4</v>
       </c>
-      <c r="L5" s="7">
+      <c r="L5" s="6">
         <f>4*7</f>
         <v>28</v>
       </c>
@@ -859,9 +922,22 @@
         <f>(SUM(C16:C19))</f>
         <v>13</v>
       </c>
-      <c r="N5" s="3"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N5" s="3">
+        <v>0</v>
+      </c>
+      <c r="O5" s="3">
+        <v>4</v>
+      </c>
+      <c r="P5" s="3">
+        <f>(SUM(E16:E19))</f>
+        <v>1.5</v>
+      </c>
+      <c r="Q5" s="3">
+        <f>(SUM(E16:E19))/4</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -884,14 +960,14 @@
       <c r="G6" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="6">
         <f>4*1</f>
         <v>4</v>
       </c>
-      <c r="L6" s="7">
+      <c r="L6" s="6">
         <f>4*7</f>
         <v>28</v>
       </c>
@@ -899,9 +975,22 @@
         <f>(SUM(C20:C23))</f>
         <v>12</v>
       </c>
-      <c r="N6" s="3"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N6" s="3">
+        <v>0</v>
+      </c>
+      <c r="O6" s="3">
+        <v>4</v>
+      </c>
+      <c r="P6" s="3">
+        <f>(SUM(E20:E23))</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="Q6" s="3">
+        <f>(SUM(E20:E23))/4</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -924,14 +1013,14 @@
       <c r="G7" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K7" s="6">
         <f>4*1</f>
         <v>4</v>
       </c>
-      <c r="L7" s="7">
+      <c r="L7" s="6">
         <f>4*7</f>
         <v>28</v>
       </c>
@@ -939,9 +1028,22 @@
         <f>(SUM(C24:C27))</f>
         <v>7</v>
       </c>
-      <c r="N7" s="3"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N7" s="3">
+        <v>0</v>
+      </c>
+      <c r="O7" s="3">
+        <v>4</v>
+      </c>
+      <c r="P7" s="3">
+        <f>(SUM(E24:E27))</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q7" s="3">
+        <f>(SUM(E24:E27))/4</f>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -958,20 +1060,20 @@
         <f t="shared" si="0"/>
         <v>0.83333333333333337</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="J8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="6">
         <f>26*1</f>
         <v>26</v>
       </c>
-      <c r="L8" s="7">
+      <c r="L8" s="6">
         <f>26*7</f>
         <v>182</v>
       </c>
@@ -979,9 +1081,22 @@
         <f>(SUM(C2:C27))</f>
         <v>112</v>
       </c>
-      <c r="N8" s="3"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N8" s="3">
+        <v>0</v>
+      </c>
+      <c r="O8" s="3">
+        <v>26</v>
+      </c>
+      <c r="P8" s="3">
+        <f>(SUM(E2:E27))</f>
+        <v>14.333333333333332</v>
+      </c>
+      <c r="Q8" s="3">
+        <f>(SUM(E2:E27))/26</f>
+        <v>0.55128205128205121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -998,15 +1113,14 @@
         <f t="shared" si="0"/>
         <v>0.83333333333333337</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="N9" s="3"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1023,14 +1137,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1047,14 +1161,14 @@
         <f t="shared" si="0"/>
         <v>0.83333333333333337</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1071,14 +1185,14 @@
         <f t="shared" si="0"/>
         <v>0.83333333333333337</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1095,14 +1209,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1119,14 +1233,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1143,14 +1257,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1167,10 +1281,10 @@
         <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="5" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1191,10 +1305,10 @@
         <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="5" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1215,10 +1329,10 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G18" s="5" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1239,10 +1353,10 @@
         <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="5" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1263,10 +1377,10 @@
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="5" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1287,10 +1401,10 @@
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F21" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="G21" s="5" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1311,10 +1425,10 @@
         <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F22" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G22" s="6" t="s">
+      <c r="G22" s="5" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1335,10 +1449,10 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G23" s="6" t="s">
+      <c r="G23" s="5" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1359,10 +1473,10 @@
         <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F24" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G24" s="6" t="s">
+      <c r="G24" s="5" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1383,10 +1497,10 @@
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F25" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G25" s="6" t="s">
+      <c r="G25" s="5" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1407,10 +1521,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="F26" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G26" s="6" t="s">
+      <c r="G26" s="5" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1431,10 +1545,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="F27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="G27" s="5" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>